<commit_message>
Updated with 12/27 game
</commit_message>
<xml_diff>
--- a/Field Days.xlsx
+++ b/Field Days.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/Desktop/Projects/Field Days/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/Desktop/Projects/Field-Days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D152A302-192D-3448-9864-3273F1FA70D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4D153D-88CE-9F45-9764-C2961CEC8AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,25 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Stats!$A$1:$T$11</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="147">
   <si>
     <t>Date</t>
   </si>
@@ -259,6 +246,24 @@
     <t>0-2</t>
   </si>
   <si>
+    <t>Jacob, Sam G, AB, Aaron</t>
+  </si>
+  <si>
+    <t>Kiernan, Brandon, Sam S</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>PK's (3-1)</t>
+  </si>
+  <si>
+    <t>Cross (0-3)</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -316,40 +321,37 @@
     <t>(Name)</t>
   </si>
   <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>11-13</t>
-  </si>
-  <si>
-    <t>8-10</t>
-  </si>
-  <si>
-    <t>8-13</t>
-  </si>
-  <si>
-    <t>4-0</t>
+    <t>2-4</t>
+  </si>
+  <si>
+    <t>12-16</t>
+  </si>
+  <si>
+    <t>11-11</t>
+  </si>
+  <si>
+    <t>8-19</t>
   </si>
   <si>
     <t>0-1</t>
   </si>
   <si>
-    <t>8-6</t>
-  </si>
-  <si>
-    <t>32-29</t>
-  </si>
-  <si>
-    <t>25-21</t>
-  </si>
-  <si>
-    <t>34-22</t>
+    <t>8-7</t>
+  </si>
+  <si>
+    <t>33-32</t>
+  </si>
+  <si>
+    <t>28-22</t>
+  </si>
+  <si>
+    <t>34-28</t>
   </si>
   <si>
     <t>3-8</t>
   </si>
   <si>
-    <t>7-5</t>
+    <t>7-6</t>
   </si>
   <si>
     <t>Anthony</t>
@@ -361,64 +363,58 @@
     <t>0-0</t>
   </si>
   <si>
-    <t>4-8</t>
+    <t>5-8</t>
+  </si>
+  <si>
+    <t>26-32</t>
+  </si>
+  <si>
+    <t>17-27</t>
+  </si>
+  <si>
+    <t>27-29</t>
+  </si>
+  <si>
+    <t>7-3</t>
+  </si>
+  <si>
+    <t>6-5</t>
+  </si>
+  <si>
+    <t>27-32</t>
+  </si>
+  <si>
+    <t>23-20</t>
+  </si>
+  <si>
+    <t>27-25</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>3-9</t>
+  </si>
+  <si>
+    <t>36-29</t>
+  </si>
+  <si>
+    <t>29-33</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>5-7</t>
   </si>
   <si>
     <t>23-31</t>
   </si>
   <si>
-    <t>16-24</t>
-  </si>
-  <si>
-    <t>21-29</t>
-  </si>
-  <si>
-    <t>7-3</t>
-  </si>
-  <si>
-    <t>5-5</t>
-  </si>
-  <si>
-    <t>5-8</t>
-  </si>
-  <si>
-    <t>27-32</t>
-  </si>
-  <si>
-    <t>23-20</t>
-  </si>
-  <si>
-    <t>27-25</t>
-  </si>
-  <si>
-    <t>5-6</t>
-  </si>
-  <si>
-    <t>3-9</t>
-  </si>
-  <si>
-    <t>35-26</t>
-  </si>
-  <si>
-    <t>29-27</t>
-  </si>
-  <si>
-    <t>6-5</t>
-  </si>
-  <si>
-    <t>6-6</t>
-  </si>
-  <si>
-    <t>4-7</t>
-  </si>
-  <si>
-    <t>20-30</t>
-  </si>
-  <si>
-    <t>13-23</t>
-  </si>
-  <si>
-    <t>17-26</t>
+    <t>14-26</t>
+  </si>
+  <si>
+    <t>23-26</t>
   </si>
   <si>
     <t>6-3</t>
@@ -430,9 +426,6 @@
     <t>1-1</t>
   </si>
   <si>
-    <t>2-4</t>
-  </si>
-  <si>
     <t>2-6</t>
   </si>
   <si>
@@ -442,34 +435,31 @@
     <t>1-0</t>
   </si>
   <si>
-    <t>10-4</t>
-  </si>
-  <si>
-    <t>37-24</t>
-  </si>
-  <si>
-    <t>28-18</t>
-  </si>
-  <si>
-    <t>30-26</t>
-  </si>
-  <si>
-    <t>3-4</t>
-  </si>
-  <si>
-    <t>13-16</t>
-  </si>
-  <si>
-    <t>14-12</t>
-  </si>
-  <si>
-    <t>16-12</t>
+    <t>10-5</t>
+  </si>
+  <si>
+    <t>38-27</t>
+  </si>
+  <si>
+    <t>31-19</t>
+  </si>
+  <si>
+    <t>30-32</t>
+  </si>
+  <si>
+    <t>4-4</t>
+  </si>
+  <si>
+    <t>16-17</t>
+  </si>
+  <si>
+    <t>15-15</t>
+  </si>
+  <si>
+    <t>22-12</t>
   </si>
   <si>
     <t>0-6</t>
-  </si>
-  <si>
-    <t>1-3</t>
   </si>
   <si>
     <t>Tighe</t>
@@ -522,16 +512,16 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -560,7 +550,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -651,6 +641,26 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -669,7 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -780,19 +790,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,9 +906,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Stats!$A$2:$A$10</c:f>
+              <c:f>Stats!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Aaron</c:v>
                 </c:pt>
@@ -922,49 +935,61 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sam G</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sam S</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Tighe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Stats!$C$2:$C$10</c:f>
+              <c:f>Stats!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.33329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57140000000000002</c:v>
+                  <c:v>0.5333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33329999999999999</c:v>
+                  <c:v>0.3846</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.3846</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.57140000000000002</c:v>
+                  <c:v>0.5333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36359999999999998</c:v>
+                  <c:v>0.41670000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.71430000000000005</c:v>
+                  <c:v>0.66669999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9F86-C340-B540-9A4440D30C0F}"/>
+              <c16:uniqueId val="{00000000-0FD0-BE47-BC92-39740177917D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -986,9 +1011,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Stats!$A$2:$A$10</c:f>
+              <c:f>Stats!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Aaron</c:v>
                 </c:pt>
@@ -1015,49 +1040,61 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sam G</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sam S</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Tighe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Stats!$E$2:$E$10</c:f>
+              <c:f>Stats!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.45829999999999999</c:v>
+                  <c:v>0.42859999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.52459999999999996</c:v>
+                  <c:v>0.50770000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.33329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4259</c:v>
+                  <c:v>0.44829999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.45760000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.57379999999999998</c:v>
+                  <c:v>0.55379999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4</c:v>
+                  <c:v>0.4259</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.45450000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.60660000000000003</c:v>
+                  <c:v>0.58460000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.48480000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.45450000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9F86-C340-B540-9A4440D30C0F}"/>
+              <c16:uniqueId val="{00000001-0FD0-BE47-BC92-39740177917D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1079,9 +1116,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Stats!$A$2:$A$10</c:f>
+              <c:f>Stats!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Aaron</c:v>
                 </c:pt>
@@ -1108,49 +1145,61 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sam G</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sam S</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Tighe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Stats!$G$2:$G$10</c:f>
+              <c:f>Stats!$G$2:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.44440000000000002</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54349999999999998</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.33329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4</c:v>
+                  <c:v>0.38640000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.53490000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.54349999999999998</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36109999999999998</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.33329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.60870000000000002</c:v>
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9F86-C340-B540-9A4440D30C0F}"/>
+              <c16:uniqueId val="{00000002-0FD0-BE47-BC92-39740177917D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1172,9 +1221,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Stats!$A$2:$A$10</c:f>
+              <c:f>Stats!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Aaron</c:v>
                 </c:pt>
@@ -1201,49 +1250,61 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sam G</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sam S</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Tighe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Stats!$I$2:$I$10</c:f>
+              <c:f>Stats!$I$2:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.38100000000000001</c:v>
+                  <c:v>0.29630000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60709999999999997</c:v>
+                  <c:v>0.5484</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42</c:v>
+                  <c:v>0.48209999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.51919999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51790000000000003</c:v>
+                  <c:v>0.4677</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39529999999999998</c:v>
+                  <c:v>0.46939999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.53569999999999995</c:v>
+                  <c:v>0.4839</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.64710000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-9F86-C340-B540-9A4440D30C0F}"/>
+              <c16:uniqueId val="{00000003-0FD0-BE47-BC92-39740177917D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1265,9 +1326,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Stats!$A$2:$A$10</c:f>
+              <c:f>Stats!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Aaron</c:v>
                 </c:pt>
@@ -1294,16 +1355,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sam G</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sam S</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Tighe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Stats!$K$2:$K$10</c:f>
+              <c:f>Stats!$K$2:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.75</c:v>
                 </c:pt>
@@ -1330,13 +1397,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.45450000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-9F86-C340-B540-9A4440D30C0F}"/>
+              <c16:uniqueId val="{00000004-0FD0-BE47-BC92-39740177917D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1358,9 +1431,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Stats!$A$2:$A$10</c:f>
+              <c:f>Stats!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Aaron</c:v>
                 </c:pt>
@@ -1387,49 +1460,61 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sam G</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sam S</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Tighe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Stats!$M$2:$M$10</c:f>
+              <c:f>Stats!$M$2:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58330000000000004</c:v>
+                  <c:v>0.53849999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0.54549999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0.46150000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.54549999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.58330000000000004</c:v>
+                  <c:v>0.53849999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.66669999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-9F86-C340-B540-9A4440D30C0F}"/>
+              <c16:uniqueId val="{00000005-0FD0-BE47-BC92-39740177917D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1453,9 +1538,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Stats!$A$2:$A$10</c:f>
+              <c:f>Stats!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Aaron</c:v>
                 </c:pt>
@@ -1482,16 +1567,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sam G</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sam S</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Tighe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Stats!$O$2:$O$10</c:f>
+              <c:f>Stats!$O$2:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1518,13 +1609,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-9F86-C340-B540-9A4440D30C0F}"/>
+              <c16:uniqueId val="{00000006-0FD0-BE47-BC92-39740177917D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1540,6 +1637,47 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Stats!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Aaron</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Anthony</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Brandon</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Eric</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Kiernan</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quinn</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sam G</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sam S</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Tighe</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Stats!$Q$2:$Q$10</c:f>
@@ -1578,7 +1716,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-9F86-C340-B540-9A4440D30C0F}"/>
+              <c16:uniqueId val="{00000007-0FD0-BE47-BC92-39740177917D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1658,9 +1796,8 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:prstDash val="solid"/>
@@ -1668,6 +1805,18 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1940,10 +2089,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:prstDash val="solid"/>
       <a:round/>
@@ -1961,16 +2107,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3428</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>3138</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>863599</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>16933</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2298,7 +2444,7 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2857,17 +3003,39 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="A16" s="6">
+        <v>45653</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
+      <c r="L16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
@@ -3153,7 +3321,7 @@
   <dimension ref="A1:AA29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3165,99 +3333,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="42" t="s">
+      <c r="A1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="C1" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="D1" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="E1" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="F1" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="G1" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="42" t="s">
+      <c r="H1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="O1" s="42" t="s">
+      <c r="I1" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="J1" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="42" t="s">
+      <c r="K1" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="42" t="s">
+      <c r="L1" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="R1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="T1" s="42" t="s">
-        <v>91</v>
+      <c r="S1" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="T1" s="46" t="s">
+        <v>97</v>
       </c>
       <c r="U1" s="17"/>
       <c r="V1" s="16"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="46"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="43"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="C2" s="38">
-        <v>0.4</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E2" s="38">
-        <v>0.45829999999999999</v>
+        <v>0.42859999999999998</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G2" s="41">
-        <v>0.44440000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I2" s="41">
-        <v>0.38100000000000001</v>
+        <v>0.29630000000000001</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>62</v>
@@ -3266,31 +3434,31 @@
         <v>0.75</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="M2" s="41">
+        <v>0.8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2" s="41">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="38">
+        <v>0</v>
+      </c>
+      <c r="R2" s="44">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="O2" s="41">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q2" s="38">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1">
-        <v>0</v>
-      </c>
       <c r="T2" s="21" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="U2" s="18"/>
     </row>
@@ -3299,40 +3467,40 @@
         <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C3" s="38">
-        <v>0.57140000000000002</v>
+        <v>0.5333</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E3" s="41">
-        <v>0.52459999999999996</v>
+        <v>0.50770000000000004</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G3" s="41">
-        <v>0.54349999999999998</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="I3" s="41">
-        <v>0.60709999999999997</v>
+        <v>0.5484</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="K3" s="41">
         <v>0.2727</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M3" s="41">
-        <v>0.58330000000000004</v>
+        <v>0.53849999999999998</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>33</v>
@@ -3346,7 +3514,7 @@
       <c r="Q3" s="38">
         <v>0.33329999999999999</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="44">
         <v>1</v>
       </c>
       <c r="S3" s="1">
@@ -3359,10 +3527,10 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C4" s="38">
         <v>0</v>
@@ -3380,43 +3548,43 @@
         <v>0.33329999999999999</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="I4" s="41">
         <v>0.6</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="K4" s="41">
         <v>0</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="M4" s="41">
         <v>0</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="O4" s="41">
         <v>0</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="Q4" s="38">
         <v>0</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="44">
         <v>0</v>
       </c>
       <c r="S4" s="1">
         <v>0</v>
       </c>
       <c r="T4" s="22" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="U4" s="18"/>
     </row>
@@ -3425,40 +3593,40 @@
         <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C5" s="38">
-        <v>0.33329999999999999</v>
+        <v>0.3846</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E5" s="41">
-        <v>0.4259</v>
+        <v>0.44829999999999998</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G5" s="41">
-        <v>0.4</v>
+        <v>0.38640000000000002</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="I5" s="41">
-        <v>0.42</v>
+        <v>0.48209999999999997</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="K5" s="41">
         <v>0.7</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="M5" s="41">
-        <v>0.5</v>
+        <v>0.54549999999999998</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>60</v>
@@ -3472,8 +3640,8 @@
       <c r="Q5" s="38">
         <v>0.33329999999999999</v>
       </c>
-      <c r="R5" s="1">
-        <v>4</v>
+      <c r="R5" s="44">
+        <v>5</v>
       </c>
       <c r="S5" s="1">
         <v>2</v>
@@ -3488,37 +3656,37 @@
         <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="38">
         <v>0.3846</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E6" s="41">
         <v>0.45760000000000001</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G6" s="41">
         <v>0.53490000000000004</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="I6" s="41">
         <v>0.51919999999999999</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="K6" s="41">
         <v>0.45450000000000002</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="M6" s="41">
         <v>0.25</v>
@@ -3535,7 +3703,7 @@
       <c r="Q6" s="38">
         <v>0.33329999999999999</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="44">
         <v>2</v>
       </c>
       <c r="S6" s="1">
@@ -3551,40 +3719,40 @@
         <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C7" s="38">
-        <v>0.57140000000000002</v>
+        <v>0.5333</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E7" s="41">
-        <v>0.57379999999999998</v>
+        <v>0.55379999999999996</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G7" s="41">
-        <v>0.54349999999999998</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="I7" s="41">
-        <v>0.51790000000000003</v>
+        <v>0.4677</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K7" s="41">
         <v>0.54549999999999998</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="M7" s="41">
-        <v>0.5</v>
+        <v>0.46150000000000002</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>60</v>
@@ -3598,7 +3766,7 @@
       <c r="Q7" s="38">
         <v>1</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="44">
         <v>1</v>
       </c>
       <c r="S7" s="1">
@@ -3614,40 +3782,40 @@
         <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C8" s="38">
-        <v>0.36359999999999998</v>
+        <v>0.41670000000000001</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E8" s="41">
-        <v>0.4</v>
+        <v>0.4259</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G8" s="41">
-        <v>0.36109999999999998</v>
+        <v>0.35</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I8" s="41">
-        <v>0.39529999999999998</v>
+        <v>0.46939999999999998</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="K8" s="41">
         <v>0.66669999999999996</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="M8" s="41">
-        <v>0.5</v>
+        <v>0.54549999999999998</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>60</v>
@@ -3661,7 +3829,7 @@
       <c r="Q8" s="38">
         <v>0.33329999999999999</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="44">
         <v>1</v>
       </c>
       <c r="S8" s="1">
@@ -3674,34 +3842,34 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C9" s="38">
         <v>0.5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E9" s="41">
         <v>0.45450000000000002</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="G9" s="41">
         <v>0.33329999999999999</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I9" s="41">
         <v>0.25</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K9" s="41">
         <v>1</v>
@@ -3713,25 +3881,25 @@
         <v>0</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="O9" s="41">
         <v>1</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="Q9" s="38">
         <v>1</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="44">
         <v>0</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
       </c>
       <c r="T9" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="U9" s="18"/>
     </row>
@@ -3740,40 +3908,40 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C10" s="38">
-        <v>0.71430000000000005</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E10" s="41">
-        <v>0.60660000000000003</v>
+        <v>0.58460000000000001</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G10" s="41">
-        <v>0.60870000000000002</v>
+        <v>0.62</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I10" s="41">
-        <v>0.53569999999999995</v>
+        <v>0.4839</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="K10" s="41">
         <v>0.45450000000000002</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M10" s="41">
-        <v>0.58330000000000004</v>
+        <v>0.53849999999999998</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>33</v>
@@ -3787,7 +3955,7 @@
       <c r="Q10" s="38">
         <v>0.66669999999999996</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="44">
         <v>4</v>
       </c>
       <c r="S10" s="20">
@@ -3803,54 +3971,54 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C11" s="39">
-        <v>0.42859999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E11" s="39">
-        <v>0.44829999999999998</v>
+        <v>0.48480000000000001</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G11" s="39">
-        <v>0.53849999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I11" s="39">
-        <v>0.57140000000000002</v>
+        <v>0.64710000000000001</v>
       </c>
       <c r="J11" s="33" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K11" s="39">
         <v>0</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="M11" s="39">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="N11" s="33" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="O11" s="39">
         <v>0.5</v>
       </c>
       <c r="P11" s="33" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="Q11" s="39">
         <v>0</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="44">
         <v>1</v>
       </c>
       <c r="S11" s="1">
@@ -3862,22 +4030,22 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C12" s="40">
         <v>0.5</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E12" s="40">
         <v>0.45450000000000002</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G12" s="40">
         <v>0.375</v>
@@ -3889,7 +4057,7 @@
         <v>0.4</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="K12" s="40">
         <v>0.5</v>
@@ -3901,25 +4069,25 @@
         <v>0.66669999999999996</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="O12" s="40">
         <v>0.5</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="Q12" s="40">
         <v>0</v>
       </c>
-      <c r="R12" s="13">
+      <c r="R12" s="45">
         <v>0</v>
       </c>
       <c r="S12" s="13">
         <v>0</v>
       </c>
       <c r="T12" s="37" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
@@ -4009,7 +4177,7 @@
       <c r="AA24" s="1"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="X25" s="44"/>
+      <c r="X25" s="42"/>
       <c r="Y25" s="39"/>
       <c r="Z25" s="38"/>
       <c r="AA25" s="1"/>
@@ -4036,7 +4204,79 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:T11" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <conditionalFormatting sqref="R2:R12">
+  <conditionalFormatting sqref="C2:C12">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E12">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G12">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I12">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K12">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M12">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4048,8 +4288,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R12">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S2:S12">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4070,58 +4334,58 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="42" t="s">
+      <c r="A1" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="42" t="s">
+      <c r="D1" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="J1" s="42" t="s">
+      <c r="I1" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="42" t="s">
-        <v>144</v>
+      <c r="L1" s="46" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B2" s="31">
         <v>0</v>
       </c>
       <c r="C2" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="32">
         <v>0</v>
@@ -4133,7 +4397,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" s="32">
         <v>2</v>
@@ -4142,7 +4406,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K2" s="32">
         <v>0</v>
@@ -4156,7 +4420,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="31">
         <v>0</v>
@@ -4171,7 +4435,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="32">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H3" s="32">
         <v>4</v>
@@ -4180,7 +4444,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K3" s="32">
         <v>5</v>
@@ -4191,7 +4455,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B4" s="32">
         <v>0</v>
@@ -4250,7 +4514,7 @@
         <v>6</v>
       </c>
       <c r="H5" s="32">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I5" s="32">
         <v>2</v>
@@ -4259,7 +4523,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L5" s="32">
         <v>1</v>
@@ -4308,10 +4572,10 @@
         <v>43</v>
       </c>
       <c r="B7" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="32">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="32">
         <v>0</v>
@@ -4332,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="32">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K7" s="32">
         <v>2</v>
@@ -4355,7 +4619,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="32">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8" s="32">
         <v>5</v>
@@ -4373,7 +4637,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L8" s="32">
         <v>2</v>
@@ -4381,7 +4645,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B9" s="32">
         <v>0</v>
@@ -4422,10 +4686,10 @@
         <v>22</v>
       </c>
       <c r="B10" s="32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" s="32">
         <v>1</v>
@@ -4437,7 +4701,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="32">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H10" s="32">
         <v>1</v>
@@ -4469,7 +4733,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="32">
         <v>4</v>
@@ -4478,7 +4742,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" s="32">
         <v>0</v>
@@ -4495,7 +4759,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B12" s="32">
         <v>0</v>
@@ -4557,7 +4821,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:K12 L11 B11:J11 K10:L10 B10:I10 J9:L9 B9:H9 I8:L8 B8:G8 H7:L7 B7:F7 G6:L6 B6:E6 F5:L5 B5:D5 E4:L4 B4:C4 D3:L3 B3 C2:L2">
+  <conditionalFormatting sqref="B4:C4 B3 B5:D5 B6:E6 B7:F7 B8:G8 B9:H9 B10:I10 B11:J11 B12:K12 C2:L2 D3:L3 E4:L4 F5:L5 G6:L6 H7:L7 I8:L8 J9:L9 K10:L10 L11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4569,7 +4833,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C12 C2 B3 D3:L3">
+  <conditionalFormatting sqref="B4:C4 D2:D3 D5:D12 E4:L4">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:D5 E2:E4 E6:E12 F5:L5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2 B3 C4:C12 D3:L3">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4581,32 +4869,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C12 D3:L3 C2">
+  <conditionalFormatting sqref="C4:C12 C2 D3:L3">
     <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D12 E4:L4 D2:D3 B4:C4">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6:E12 E2:E4 F5:L5 B5:D5">
-    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>